<commit_message>
added KOOP xlsx parameters
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KOOP/props/KOOP.xlsx
+++ b/src/main/resources/input/KOOP/props/KOOP.xlsx
@@ -1332,10 +1332,10 @@
   <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2108,13 +2108,13 @@
         <v>16</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Parameter checktvmissing replaced by checktvoccurs https://github.com/Imvertor/Imvertor-Maven/issues/25
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KOOP/props/KOOP.xlsx
+++ b/src/main/resources/input/KOOP/props/KOOP.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="285">
   <si>
     <t>Name</t>
   </si>
@@ -414,9 +414,6 @@
     <t>Check if tagged values are assigned correctly</t>
   </si>
   <si>
-    <t>validatetvmissing</t>
-  </si>
-  <si>
     <t>Check if tagged values that are required are specified</t>
   </si>
   <si>
@@ -880,6 +877,9 @@
   </si>
   <si>
     <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>validatetvoccurs</t>
   </si>
 </sst>
 </file>
@@ -1332,10 +1332,10 @@
   <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="A92" sqref="A92:XFD92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1365,46 +1365,46 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>249</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>54</v>
@@ -1413,13 +1413,13 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1448,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1471,18 +1471,18 @@
         <v>4</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="D6" s="7" t="b">
         <v>0</v>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1519,13 +1519,13 @@
     </row>
     <row r="9" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="D9" s="7" t="b">
         <v>0</v>
@@ -1557,18 +1557,18 @@
         <v>4</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>0</v>
@@ -1579,14 +1579,14 @@
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1620,7 +1620,7 @@
         <v>16</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -1646,13 +1646,13 @@
         <v>19</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1677,27 +1677,27 @@
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1708,18 +1708,18 @@
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
@@ -1730,14 +1730,14 @@
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
       </c>
@@ -1745,19 +1745,19 @@
         <v>1</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
@@ -1765,18 +1765,18 @@
         <v>1</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="23" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
@@ -1921,18 +1921,18 @@
         <v>4</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
@@ -1973,18 +1973,18 @@
         <v>34</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="D29" s="2" t="b">
         <v>0</v>
@@ -1995,13 +1995,13 @@
     </row>
     <row r="30" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
@@ -2119,13 +2119,13 @@
     </row>
     <row r="35" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
@@ -2157,7 +2157,7 @@
         <v>16</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2177,10 +2177,10 @@
         <v>0</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2211,13 +2211,13 @@
     </row>
     <row r="40" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="D40" s="2" t="b">
         <v>0</v>
@@ -2260,16 +2260,16 @@
         <v>1</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G42" s="6"/>
       <c r="L42" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -2281,19 +2281,19 @@
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>182</v>
-      </c>
       <c r="D44" s="7" t="b">
         <v>0</v>
       </c>
@@ -2304,19 +2304,19 @@
         <v>4</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="D45" s="7" t="b">
         <v>0</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2387,18 +2387,18 @@
         <v>16</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="D49" s="2" t="b">
         <v>0</v>
@@ -2412,30 +2412,30 @@
     </row>
     <row r="50" spans="1:12" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>189</v>
-      </c>
       <c r="D50" s="7" t="b">
         <v>0</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="D51" s="7" t="b">
         <v>0</v>
@@ -2447,7 +2447,7 @@
         <v>19</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2467,10 +2467,10 @@
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="L52" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2490,10 +2490,10 @@
         <v>0</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L53" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2504,7 +2504,7 @@
         <v>69</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D54" s="2" t="b">
         <v>0</v>
@@ -2513,10 +2513,10 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -2536,22 +2536,22 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="D56" s="2" t="b">
         <v>0</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2579,18 +2579,18 @@
         <v>0</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="D58" s="2" t="b">
         <v>0</v>
@@ -2622,18 +2622,18 @@
         <v>16</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>1</v>
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2722,21 +2722,21 @@
         <v>0</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="D65" s="2" t="b">
         <v>0</v>
@@ -2750,14 +2750,14 @@
     </row>
     <row r="66" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="D66" s="7" t="b">
         <v>0</v>
       </c>
@@ -2765,10 +2765,10 @@
         <v>1</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2788,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="68" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2831,19 +2831,19 @@
         <v>92</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A70" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>151</v>
-      </c>
       <c r="D70" s="7" t="b">
         <v>0</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>4</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:12" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
@@ -2879,7 +2879,7 @@
     </row>
     <row r="72" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -2904,14 +2904,14 @@
     </row>
     <row r="73" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2942,21 +2942,21 @@
         <v>0</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="76" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -2978,7 +2978,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="77" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3018,10 +3018,10 @@
         <v>1</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3046,14 +3046,14 @@
     </row>
     <row r="80" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="D80" s="2" t="b">
         <v>0</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>1</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:12" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
@@ -3084,7 +3084,7 @@
         <v>107</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3104,10 +3104,10 @@
         <v>0</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -3127,10 +3127,10 @@
         <v>0</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L83" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -3150,10 +3150,10 @@
         <v>0</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L84" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="85" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -3176,7 +3176,7 @@
         <v>16</v>
       </c>
       <c r="L85" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3268,13 +3268,13 @@
     </row>
     <row r="89" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="D89" s="2" t="b">
         <v>0</v>
@@ -3315,7 +3315,7 @@
         <v>16</v>
       </c>
       <c r="L90" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3347,19 +3347,19 @@
         <v>4</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="D92" s="2" t="b">
         <v>1</v>
       </c>
@@ -3377,20 +3377,17 @@
       </c>
       <c r="K92" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="93" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D93" s="2" t="b">
         <v>1</v>
@@ -3399,19 +3396,19 @@
         <v>0</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="94" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="D94" s="2" t="b">
         <v>1</v>
       </c>
@@ -3419,10 +3416,10 @@
         <v>0</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.4">
@@ -3527,48 +3524,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Redesign of parameters excel; added BRO excel
</commit_message>
<xml_diff>
--- a/src/main/resources/input/KOOP/props/KOOP.xlsx
+++ b/src/main/resources/input/KOOP/props/KOOP.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="287">
   <si>
     <t>Name</t>
   </si>
@@ -648,15 +648,6 @@
     <t>Yes if warnings should be suppressed in documentation</t>
   </si>
   <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>uitgebreid</t>
-  </si>
-  <si>
-    <t>opleveren</t>
-  </si>
-  <si>
     <t>navragen</t>
   </si>
   <si>
@@ -880,13 +871,28 @@
   </si>
   <si>
     <t>validatetvoccurs</t>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>MIM-minimum</t>
+  </si>
+  <si>
+    <t>MIM-uitgebreid</t>
+  </si>
+  <si>
+    <t>MIM-opleveren</t>
+  </si>
+  <si>
+    <t>MIM-docrelease</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,8 +955,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -970,6 +983,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -997,15 +1015,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1032,20 +1051,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,13 +1360,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L116"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A92" sqref="A92:XFD92"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1346,15 +1377,16 @@
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="17.3828125" customWidth="1"/>
-    <col min="7" max="7" width="21.3046875" customWidth="1"/>
+    <col min="7" max="7" width="5.4609375" style="18" customWidth="1"/>
     <col min="8" max="8" width="12.69140625" customWidth="1"/>
     <col min="9" max="9" width="14.765625" customWidth="1"/>
     <col min="10" max="10" width="14.3046875" customWidth="1"/>
     <col min="11" max="11" width="15.765625" customWidth="1"/>
-    <col min="12" max="12" width="27.3046875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.07421875" style="18" customWidth="1"/>
+    <col min="13" max="13" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1365,53 +1397,51 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>247</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="G1" s="15"/>
       <c r="H1" s="4" t="s">
-        <v>248</v>
+        <v>282</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>248</v>
+        <v>282</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>248</v>
+        <v>282</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+        <v>282</v>
+      </c>
+      <c r="L1" s="15"/>
+      <c r="M1" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>277</v>
-      </c>
+      <c r="G2" s="16"/>
       <c r="H2" s="3" t="s">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>208</v>
+        <v>284</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>209</v>
+        <v>285</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+        <v>286</v>
+      </c>
+      <c r="L2" s="16"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
@@ -1427,8 +1457,10 @@
       <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G3" s="17"/>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1447,11 +1479,13 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1470,11 +1504,13 @@
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>158</v>
       </c>
@@ -1490,8 +1526,10 @@
       <c r="E6" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G6" s="17"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
@@ -1507,17 +1545,21 @@
       <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G8" s="17"/>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>161</v>
       </c>
@@ -1536,8 +1578,10 @@
       <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G9" s="17"/>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1556,11 +1600,13 @@
       <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>163</v>
       </c>
@@ -1576,8 +1622,10 @@
       <c r="E11" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G11" s="17"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>135</v>
       </c>
@@ -1596,11 +1644,13 @@
       <c r="F12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1619,11 +1669,13 @@
       <c r="F13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="G13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1639,6 +1691,7 @@
       <c r="E14" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G14" s="17"/>
       <c r="H14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1646,16 +1699,17 @@
         <v>19</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1674,16 +1728,18 @@
       <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G15" s="17"/>
+      <c r="L15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>1</v>
@@ -1692,12 +1748,14 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>251</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="L16" s="17"/>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1707,11 +1765,22 @@
       <c r="E17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G17" s="17"/>
+      <c r="H17" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="L17" s="17"/>
+    </row>
+    <row r="18" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>165</v>
       </c>
@@ -1727,8 +1796,10 @@
       <c r="E18" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G18" s="17"/>
+      <c r="L18" s="17"/>
+    </row>
+    <row r="19" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>137</v>
       </c>
@@ -1744,11 +1815,13 @@
       <c r="E19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="F19" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="L19" s="17"/>
+    </row>
+    <row r="20" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>140</v>
       </c>
@@ -1764,11 +1837,13 @@
       <c r="E20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="F20" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="L20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>143</v>
       </c>
@@ -1784,6 +1859,7 @@
       <c r="E21" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G21" s="17"/>
       <c r="H21" s="2" t="s">
         <v>16</v>
       </c>
@@ -1796,8 +1872,9 @@
       <c r="K21" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L21" s="17"/>
+    </row>
+    <row r="22" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1816,8 +1893,10 @@
       <c r="F22" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G22" s="17"/>
+      <c r="L22" s="17"/>
+    </row>
+    <row r="23" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>167</v>
       </c>
@@ -1833,8 +1912,10 @@
       <c r="E23" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="G23" s="17"/>
+      <c r="L23" s="17"/>
+    </row>
+    <row r="24" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1850,6 +1931,7 @@
       <c r="E24" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G24" s="17"/>
       <c r="H24" s="2" t="s">
         <v>16</v>
       </c>
@@ -1862,8 +1944,9 @@
       <c r="K24" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L24" s="17"/>
+    </row>
+    <row r="25" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1879,6 +1962,7 @@
       <c r="E25" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G25" s="17"/>
       <c r="H25" s="2" t="s">
         <v>16</v>
       </c>
@@ -1891,8 +1975,9 @@
       <c r="K25" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="L25" s="17"/>
+    </row>
+    <row r="26" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1908,6 +1993,7 @@
       <c r="E26" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G26" s="17"/>
       <c r="H26" s="2" t="s">
         <v>16</v>
       </c>
@@ -1920,11 +2006,12 @@
       <c r="K26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L26" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L26" s="17"/>
+      <c r="M26" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>145</v>
       </c>
@@ -1940,6 +2027,7 @@
       <c r="E27" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G27" s="17"/>
       <c r="H27" s="2" t="s">
         <v>16</v>
       </c>
@@ -1952,8 +2040,9 @@
       <c r="K27" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L27" s="17"/>
+    </row>
+    <row r="28" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1972,11 +2061,13 @@
       <c r="F28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>169</v>
       </c>
@@ -1992,8 +2083,10 @@
       <c r="E29" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G29" s="17"/>
+      <c r="L29" s="17"/>
+    </row>
+    <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>172</v>
       </c>
@@ -2009,8 +2102,10 @@
       <c r="E30" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G30" s="17"/>
+      <c r="L30" s="17"/>
+    </row>
+    <row r="31" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -2026,6 +2121,7 @@
       <c r="E31" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G31" s="17"/>
       <c r="H31" s="2" t="s">
         <v>16</v>
       </c>
@@ -2038,8 +2134,9 @@
       <c r="K31" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="L31" s="17"/>
+    </row>
+    <row r="32" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -2055,6 +2152,7 @@
       <c r="E32" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G32" s="17"/>
       <c r="H32" s="2" t="s">
         <v>16</v>
       </c>
@@ -2067,8 +2165,9 @@
       <c r="K32" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L32" s="17"/>
+    </row>
+    <row r="33" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -2087,8 +2186,10 @@
       <c r="F33" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G33" s="17"/>
+      <c r="L33" s="17"/>
+    </row>
+    <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -2104,6 +2205,7 @@
       <c r="E34" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G34" s="17"/>
       <c r="H34" s="2" t="s">
         <v>16</v>
       </c>
@@ -2116,8 +2218,9 @@
       <c r="K34" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L34" s="17"/>
+    </row>
+    <row r="35" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>175</v>
       </c>
@@ -2136,8 +2239,10 @@
       <c r="F35" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="G35" s="17"/>
+      <c r="L35" s="17"/>
+    </row>
+    <row r="36" spans="1:13" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
         <v>45</v>
       </c>
@@ -2156,11 +2261,13 @@
       <c r="F36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L36" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A37" s="7" t="s">
         <v>47</v>
       </c>
@@ -2177,13 +2284,15 @@
         <v>0</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>247</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="14" t="s">
         <v>50</v>
       </c>
@@ -2202,14 +2311,18 @@
       <c r="F38" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G38" s="17"/>
+      <c r="L38" s="17"/>
+    </row>
+    <row r="39" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
-    </row>
-    <row r="40" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G39" s="17"/>
+      <c r="L39" s="17"/>
+    </row>
+    <row r="40" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>177</v>
       </c>
@@ -2225,8 +2338,10 @@
       <c r="E40" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G40" s="17"/>
+      <c r="L40" s="17"/>
+    </row>
+    <row r="41" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>52</v>
       </c>
@@ -2242,8 +2357,10 @@
       <c r="E41" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="G41" s="17"/>
+      <c r="L41" s="17"/>
+    </row>
+    <row r="42" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>54</v>
       </c>
@@ -2260,16 +2377,17 @@
         <v>1</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G42" s="6"/>
-      <c r="L42" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>216</v>
+      </c>
+      <c r="G42" s="19"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -2280,11 +2398,22 @@
         <v>0</v>
       </c>
       <c r="F43" s="6"/>
-      <c r="G43" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G43" s="19"/>
+      <c r="H43" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="K43" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="L43" s="17"/>
+    </row>
+    <row r="44" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
         <v>180</v>
       </c>
@@ -2303,11 +2432,13 @@
       <c r="F44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L44" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>182</v>
       </c>
@@ -2324,10 +2455,12 @@
         <v>1</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>237</v>
+      </c>
+      <c r="G45" s="17"/>
+      <c r="L45" s="17"/>
+    </row>
+    <row r="46" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
@@ -2346,8 +2479,10 @@
       <c r="F46" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G46" s="17"/>
+      <c r="L46" s="17"/>
+    </row>
+    <row r="47" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
@@ -2366,8 +2501,10 @@
       <c r="F47" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="G47" s="17"/>
+      <c r="L47" s="17"/>
+    </row>
+    <row r="48" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
         <v>61</v>
       </c>
@@ -2386,11 +2523,13 @@
       <c r="F48" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L48" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>185</v>
       </c>
@@ -2409,8 +2548,10 @@
       <c r="F49" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="G49" s="17"/>
+      <c r="L49" s="17"/>
+    </row>
+    <row r="50" spans="1:13" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
         <v>187</v>
       </c>
@@ -2423,11 +2564,13 @@
       <c r="D50" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="L50" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
         <v>189</v>
       </c>
@@ -2446,11 +2589,13 @@
       <c r="F51" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L51" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>63</v>
       </c>
@@ -2467,13 +2612,15 @@
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>220</v>
+      </c>
+      <c r="G52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
         <v>65</v>
       </c>
@@ -2490,13 +2637,15 @@
         <v>0</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="L53" s="7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>247</v>
+      </c>
+      <c r="G53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>68</v>
       </c>
@@ -2513,13 +2662,15 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+        <v>238</v>
+      </c>
+      <c r="G54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>70</v>
       </c>
@@ -2536,13 +2687,15 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>280</v>
+      </c>
+      <c r="G55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>192</v>
       </c>
@@ -2559,10 +2712,12 @@
         <v>1</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>224</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="L56" s="17"/>
+    </row>
+    <row r="57" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>72</v>
       </c>
@@ -2578,11 +2733,22 @@
       <c r="E57" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G57" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G57" s="17"/>
+      <c r="H57" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J57" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="K57" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="L57" s="17"/>
+    </row>
+    <row r="58" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>195</v>
       </c>
@@ -2601,8 +2767,10 @@
       <c r="F58" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G58" s="17"/>
+      <c r="L58" s="17"/>
+    </row>
+    <row r="59" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
         <v>74</v>
       </c>
@@ -2621,19 +2789,21 @@
       <c r="F59" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L59" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>1</v>
@@ -2644,8 +2814,10 @@
       <c r="F60" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G60" s="17"/>
+      <c r="L60" s="17"/>
+    </row>
+    <row r="61" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>76</v>
       </c>
@@ -2664,8 +2836,10 @@
       <c r="F61" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G61" s="17"/>
+      <c r="L61" s="17"/>
+    </row>
+    <row r="62" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>78</v>
       </c>
@@ -2681,11 +2855,22 @@
       <c r="E62" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G62" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="G62" s="17"/>
+      <c r="H62" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J62" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="K62" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="L62" s="17"/>
+    </row>
+    <row r="63" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>80</v>
       </c>
@@ -2704,8 +2889,10 @@
       <c r="F63" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G63" s="17"/>
+      <c r="L63" s="17"/>
+    </row>
+    <row r="64" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="7" t="s">
         <v>83</v>
       </c>
@@ -2722,13 +2909,15 @@
         <v>0</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="L64" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>275</v>
+      </c>
+      <c r="G64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>197</v>
       </c>
@@ -2747,8 +2936,10 @@
       <c r="F65" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="G65" s="17"/>
+      <c r="L65" s="17"/>
+    </row>
+    <row r="66" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
         <v>200</v>
       </c>
@@ -2765,13 +2956,15 @@
         <v>1</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="L66" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>239</v>
+      </c>
+      <c r="G66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
@@ -2787,11 +2980,22 @@
       <c r="E67" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G67" s="12" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G67" s="17"/>
+      <c r="H67" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="J67" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="K67" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="L67" s="17"/>
+    </row>
+    <row r="68" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>87</v>
       </c>
@@ -2810,8 +3014,10 @@
       <c r="F68" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="G68" s="17"/>
+      <c r="L68" s="17"/>
+    </row>
+    <row r="69" spans="1:13" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A69" s="7" t="s">
         <v>91</v>
       </c>
@@ -2830,11 +3036,13 @@
       <c r="F69" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L69" s="8" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="G69" s="17"/>
+      <c r="L69" s="17"/>
+      <c r="M69" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A70" s="7" t="s">
         <v>149</v>
       </c>
@@ -2853,11 +3061,13 @@
       <c r="F70" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L70" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="G70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -2876,10 +3086,12 @@
       <c r="F71" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G71" s="17"/>
+      <c r="L71" s="17"/>
+    </row>
+    <row r="72" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -2889,6 +3101,7 @@
       <c r="E72" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G72" s="17"/>
       <c r="H72" s="2" t="s">
         <v>16</v>
       </c>
@@ -2901,8 +3114,9 @@
       <c r="K72" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L72" s="17"/>
+    </row>
+    <row r="73" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>151</v>
       </c>
@@ -2921,11 +3135,13 @@
       <c r="F73" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L73" s="8" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G73" s="17"/>
+      <c r="L73" s="17"/>
+      <c r="M73" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>98</v>
       </c>
@@ -2941,14 +3157,25 @@
       <c r="E74" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G74" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="L74" s="8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G74" s="17"/>
+      <c r="H74" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="I74" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="J74" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="K74" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="L74" s="17"/>
+      <c r="M74" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>202</v>
       </c>
@@ -2964,10 +3191,12 @@
       <c r="E75" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G75" s="17"/>
+      <c r="L75" s="17"/>
+    </row>
+    <row r="76" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -2977,11 +3206,22 @@
       <c r="E76" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G76" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G76" s="17"/>
+      <c r="H76" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="I76" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J76" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="K76" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="L76" s="17"/>
+    </row>
+    <row r="77" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>100</v>
       </c>
@@ -3000,8 +3240,10 @@
       <c r="F77" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="G77" s="17"/>
+      <c r="L77" s="17"/>
+    </row>
+    <row r="78" spans="1:13" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>102</v>
       </c>
@@ -3018,13 +3260,15 @@
         <v>1</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="L78" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>279</v>
+      </c>
+      <c r="G78" s="19"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>104</v>
       </c>
@@ -3043,8 +3287,10 @@
       <c r="F79" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G79" s="17"/>
+      <c r="L79" s="17"/>
+    </row>
+    <row r="80" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>205</v>
       </c>
@@ -3060,11 +3306,13 @@
       <c r="E80" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="L80" s="8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="G80" s="17"/>
+      <c r="L80" s="17"/>
+      <c r="M80" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>106</v>
       </c>
@@ -3083,11 +3331,13 @@
       <c r="F81" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L81" s="8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G81" s="17"/>
+      <c r="L81" s="17"/>
+      <c r="M81" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>110</v>
       </c>
@@ -3103,14 +3353,25 @@
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G82" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="L82" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="G82" s="17"/>
+      <c r="H82" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J82" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="L82" s="17"/>
+      <c r="M82" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
         <v>112</v>
       </c>
@@ -3127,13 +3388,15 @@
         <v>0</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="L83" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+        <v>247</v>
+      </c>
+      <c r="G83" s="17"/>
+      <c r="L83" s="17"/>
+      <c r="M83" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="7" t="s">
         <v>114</v>
       </c>
@@ -3150,13 +3413,15 @@
         <v>0</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="L84" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+        <v>247</v>
+      </c>
+      <c r="G84" s="17"/>
+      <c r="L84" s="17"/>
+      <c r="M84" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="7" t="s">
         <v>116</v>
       </c>
@@ -3175,11 +3440,13 @@
       <c r="F85" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L85" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G85" s="17"/>
+      <c r="L85" s="17"/>
+      <c r="M85" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>118</v>
       </c>
@@ -3195,6 +3462,7 @@
       <c r="E86" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G86" s="17"/>
       <c r="H86" s="2" t="s">
         <v>4</v>
       </c>
@@ -3207,8 +3475,9 @@
       <c r="K86" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L86" s="17"/>
+    </row>
+    <row r="87" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>120</v>
       </c>
@@ -3224,6 +3493,7 @@
       <c r="E87" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G87" s="17"/>
       <c r="H87" s="2" t="s">
         <v>4</v>
       </c>
@@ -3236,8 +3506,9 @@
       <c r="K87" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L87" s="17"/>
+    </row>
+    <row r="88" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>122</v>
       </c>
@@ -3253,6 +3524,7 @@
       <c r="E88" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G88" s="17"/>
       <c r="H88" s="2" t="s">
         <v>16</v>
       </c>
@@ -3265,8 +3537,9 @@
       <c r="K88" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L88" s="17"/>
+    </row>
+    <row r="89" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>153</v>
       </c>
@@ -3282,6 +3555,7 @@
       <c r="E89" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G89" s="17"/>
       <c r="H89" s="2" t="s">
         <v>16</v>
       </c>
@@ -3294,8 +3568,9 @@
       <c r="K89" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L89" s="17"/>
+    </row>
+    <row r="90" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="7" t="s">
         <v>124</v>
       </c>
@@ -3314,11 +3589,13 @@
       <c r="F90" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L90" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="G90" s="17"/>
+      <c r="L90" s="17"/>
+      <c r="M90" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>127</v>
       </c>
@@ -3334,6 +3611,7 @@
       <c r="E91" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G91" s="17"/>
       <c r="H91" s="2" t="s">
         <v>16</v>
       </c>
@@ -3346,13 +3624,14 @@
       <c r="K91" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L91" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L91" s="17"/>
+      <c r="M91" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>5</v>
@@ -3366,6 +3645,7 @@
       <c r="E92" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="G92" s="17"/>
       <c r="H92" s="2" t="s">
         <v>16</v>
       </c>
@@ -3378,8 +3658,9 @@
       <c r="K92" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L92" s="17"/>
+    </row>
+    <row r="93" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>130</v>
       </c>
@@ -3395,11 +3676,22 @@
       <c r="E93" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G93" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="G93" s="17"/>
+      <c r="H93" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="I93" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="J93" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="K93" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="L93" s="17"/>
+    </row>
+    <row r="94" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>132</v>
       </c>
@@ -3416,77 +3708,79 @@
         <v>0</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="L94" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L95"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L96"/>
-    </row>
-    <row r="97" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L97"/>
-    </row>
-    <row r="98" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L98"/>
-    </row>
-    <row r="99" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L99"/>
-    </row>
-    <row r="100" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L100"/>
-    </row>
-    <row r="101" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L101"/>
-    </row>
-    <row r="102" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L102"/>
-    </row>
-    <row r="103" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L103"/>
-    </row>
-    <row r="104" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L104"/>
-    </row>
-    <row r="105" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L105"/>
-    </row>
-    <row r="106" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L106"/>
-    </row>
-    <row r="107" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L107"/>
-    </row>
-    <row r="108" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L108"/>
-    </row>
-    <row r="109" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L109"/>
-    </row>
-    <row r="110" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L110"/>
-    </row>
-    <row r="111" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L111"/>
-    </row>
-    <row r="112" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L112"/>
-    </row>
-    <row r="113" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L113"/>
-    </row>
-    <row r="114" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L114"/>
-    </row>
-    <row r="115" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L115"/>
-    </row>
-    <row r="116" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L116"/>
+        <v>257</v>
+      </c>
+      <c r="G94" s="17"/>
+      <c r="L94" s="17"/>
+      <c r="M94" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M95"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M96"/>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M97"/>
+    </row>
+    <row r="98" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M98"/>
+    </row>
+    <row r="99" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M99"/>
+    </row>
+    <row r="100" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M100"/>
+    </row>
+    <row r="101" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M101"/>
+    </row>
+    <row r="102" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M102"/>
+    </row>
+    <row r="103" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M103"/>
+    </row>
+    <row r="104" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M104"/>
+    </row>
+    <row r="105" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M105"/>
+    </row>
+    <row r="106" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M106"/>
+    </row>
+    <row r="107" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M107"/>
+    </row>
+    <row r="108" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M108"/>
+    </row>
+    <row r="109" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M109"/>
+    </row>
+    <row r="110" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M110"/>
+    </row>
+    <row r="111" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M111"/>
+    </row>
+    <row r="112" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M112"/>
+    </row>
+    <row r="113" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M113"/>
+    </row>
+    <row r="114" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M114"/>
+    </row>
+    <row r="115" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M115"/>
+    </row>
+    <row r="116" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M116"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3524,48 +3818,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>